<commit_message>
add new column refseq_orientation_match; fix bug when no sample location given
</commit_message>
<xml_diff>
--- a/data/submission_spreadsheets/SRP198941_SLX15021_GEP00005.xlsx
+++ b/data/submission_spreadsheets/SRP198941_SLX15021_GEP00005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="17520" tabRatio="736"/>
+    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="17520" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8340" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8343" uniqueCount="1240">
   <si>
     <t>description</t>
   </si>
@@ -4242,6 +4242,28 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> is a list of sequences that the reads are counted against. If looking for particular gene edits, the desired edited sequences should be put in here. If no sequence is provided, the amplicon as identified by the provided primer sequences will be considered for counting reads</t>
+    </r>
+  </si>
+  <si>
+    <t>refseq_orientation_match</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[optional]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Is the orientation of the amplicon match the NCBI whole genome reference sequence (RefSeq)? (TRUE/FALSE) Default set to True. Please consult the schematic drawing on the amplicon tab for more details.</t>
     </r>
   </si>
 </sst>
@@ -4968,7 +4990,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="132">
+  <dxfs count="133">
     <dxf>
       <font>
         <b val="0"/>
@@ -5671,6 +5693,23 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -7189,9 +7228,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table246" displayName="Table246" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="131"/>
-    <tableColumn id="2" name="Column names" dataDxfId="130"/>
-    <tableColumn id="3" name="Description" dataDxfId="129"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="132"/>
+    <tableColumn id="2" name="Column names" dataDxfId="131"/>
+    <tableColumn id="3" name="Description" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7200,97 +7239,98 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table5061" displayName="Table5061" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="94" dataDxfId="93"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="92" dataDxfId="91"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="90" dataDxfId="89"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="95" dataDxfId="94"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="93" dataDxfId="92"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="91" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table1262" displayName="Table1262" ref="A73:C76" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table1262" displayName="Table1262" ref="A74:C77" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="88"/>
-    <tableColumn id="2" name="Column names" dataDxfId="87"/>
-    <tableColumn id="3" name="Description" dataDxfId="86"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="89"/>
+    <tableColumn id="2" name="Column names" dataDxfId="88"/>
+    <tableColumn id="3" name="Description" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="83"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="82"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="81"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="80"/>
-    <tableColumn id="5" name="target_start" dataDxfId="79"/>
-    <tableColumn id="6" name="target_end" dataDxfId="78"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="77"/>
+    <tableColumn id="1" name="target_name" dataDxfId="84"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="83"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="82"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="81"/>
+    <tableColumn id="5" name="target_start" dataDxfId="80"/>
+    <tableColumn id="6" name="target_end" dataDxfId="79"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="74"/>
+    <tableColumn id="1" name="target_description" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="71"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="70"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="69"/>
+    <tableColumn id="1" name="target_name" dataDxfId="72"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="71"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="66"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="65"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="64"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="63"/>
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="67"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="66"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="65"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:N9" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:N9" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <tableColumns count="14">
-    <tableColumn id="14" name="amplicon_name" dataDxfId="60"/>
-    <tableColumn id="1" name="guide_name" dataDxfId="59"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="58"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="57"/>
-    <tableColumn id="4" name="guide_strand" dataDxfId="56"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="55"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="54"/>
-    <tableColumn id="7" name="chrom" dataDxfId="53"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="52"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="51"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="50"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="49"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="48"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="47"/>
+    <tableColumn id="14" name="amplicon_name" dataDxfId="61"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="60"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="59"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="58"/>
+    <tableColumn id="4" name="guide_strand" dataDxfId="57"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="56"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="55"/>
+    <tableColumn id="7" name="chrom" dataDxfId="54"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="53"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="52"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="51"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="50"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="49"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="O1:P9" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="O1:Q9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <tableColumns count="3">
+    <tableColumn id="3" name="refseq_orientation_match" dataDxfId="45"/>
     <tableColumn id="1" name="score" dataDxfId="44"/>
     <tableColumn id="2" name="description" dataDxfId="43"/>
   </tableColumns>
@@ -7330,9 +7370,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table353" displayName="Table353" ref="A14:C18" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="128"/>
-    <tableColumn id="2" name="Column names" dataDxfId="127"/>
-    <tableColumn id="3" name="Description" dataDxfId="126"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="129"/>
+    <tableColumn id="2" name="Column names" dataDxfId="128"/>
+    <tableColumn id="3" name="Description" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7389,11 +7429,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table454" displayName="Table454" ref="A67:C72" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table454" displayName="Table454" ref="A68:C73" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="125"/>
-    <tableColumn id="2" name="Column names" dataDxfId="124"/>
-    <tableColumn id="3" name="Description" dataDxfId="123"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="126"/>
+    <tableColumn id="2" name="Column names" dataDxfId="125"/>
+    <tableColumn id="3" name="Description" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7402,53 +7442,53 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table555" displayName="Table555" ref="A23:C36" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="122"/>
-    <tableColumn id="2" name="Column names" dataDxfId="121"/>
-    <tableColumn id="3" name="Description" dataDxfId="120"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="123"/>
+    <tableColumn id="2" name="Column names" dataDxfId="122"/>
+    <tableColumn id="3" name="Description" dataDxfId="121"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table656" displayName="Table656" ref="A39:C43" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table656" displayName="Table656" ref="A40:C44" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="119"/>
-    <tableColumn id="2" name="Column names" dataDxfId="118"/>
-    <tableColumn id="3" name="Description" dataDxfId="117"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="120"/>
+    <tableColumn id="2" name="Column names" dataDxfId="119"/>
+    <tableColumn id="3" name="Description" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table757" displayName="Table757" ref="A61:C66" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table757" displayName="Table757" ref="A62:C67" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="116"/>
-    <tableColumn id="2" name="Column names" dataDxfId="115"/>
-    <tableColumn id="3" name="Description" dataDxfId="114"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="117"/>
+    <tableColumn id="2" name="Column names" dataDxfId="116"/>
+    <tableColumn id="3" name="Description" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table4758" displayName="Table4758" ref="A44:C60" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table4758" displayName="Table4758" ref="A45:C61" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="113" dataDxfId="112"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="111" dataDxfId="110"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="109" dataDxfId="108"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="114" dataDxfId="113"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="112" dataDxfId="111"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="110" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table4859" displayName="Table4859" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="107" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table4859" displayName="Table4859" ref="A37:C39" headerRowCount="0" totalsRowShown="0" dataDxfId="108" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="106" dataDxfId="105" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="104" dataDxfId="103" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="102" dataDxfId="101" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="107" dataDxfId="106" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="105" dataDxfId="104" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="103" dataDxfId="102" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7457,9 +7497,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table4960" displayName="Table4960" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="100" dataDxfId="99"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="98" dataDxfId="97"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="96" dataDxfId="95"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="101" dataDxfId="100"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="99" dataDxfId="98"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="97" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7790,9 +7830,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -8102,322 +8142,331 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
-      <c r="A37" s="2"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="3" t="s">
-        <v>11</v>
+        <v>1238</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>232</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:3" ht="30">
+      <c r="A41" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="B41" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" s="3" t="s">
-        <v>20</v>
+        <v>235</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>225</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" s="3" t="s">
-        <v>189</v>
+        <v>28</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="3" t="s">
-        <v>29</v>
+        <v>190</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="3" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="3" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="B49" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="B50" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="B51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="B52" s="3"/>
-      <c r="C52" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" s="3"/>
       <c r="C53" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="3"/>
       <c r="C54" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="3"/>
       <c r="C55" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="3"/>
       <c r="C56" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="B57" s="3"/>
       <c r="C57" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="30" customHeight="1">
       <c r="B58" s="3"/>
       <c r="C58" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" s="3"/>
+      <c r="C59" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="45">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" ht="45">
+      <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C63" s="13" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="B63" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30" customHeight="1">
       <c r="B64" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" s="3" t="s">
-        <v>27</v>
+        <v>237</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="B69" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>76</v>
+        <v>398</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="B71" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="B72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="45">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:3" ht="45">
+      <c r="A75" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C75" s="13" t="s">
         <v>1237</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="B75" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="B76" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>396</v>
       </c>
     </row>
@@ -8458,7 +8507,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9079,9 +9128,12 @@
         <v>19</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9128,10 +9180,10 @@
       <c r="N2" s="14">
         <v>53704310</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -9178,10 +9230,10 @@
       <c r="N3" s="14">
         <v>53700865</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="Q3" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -9228,10 +9280,10 @@
       <c r="N4" s="14">
         <v>44344605</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="Q4" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -9278,10 +9330,10 @@
       <c r="N5" s="14">
         <v>54285936</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="Q5" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9328,10 +9380,10 @@
       <c r="N6" s="14">
         <v>54931395</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9378,7 +9430,7 @@
       <c r="N7" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="Q7" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9425,7 +9477,7 @@
       <c r="N8" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="Q8" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9472,7 +9524,7 @@
       <c r="N9" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="Q9" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9540,7 +9592,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$C$2:$C$4</xm:f>
@@ -9558,6 +9610,12 @@
             <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>E10:E1048576 F2:F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Menus!D2:D3</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add new amplicon diagram to submission spreadsheet; fix issue of using differents amplicon id for target search and amplicount
</commit_message>
<xml_diff>
--- a/data/submission_spreadsheets/SRP198941_SLX15021_GEP00005.xlsx
+++ b/data/submission_spreadsheets/SRP198941_SLX15021_GEP00005.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="7600" windowWidth="25600" windowHeight="9380" tabRatio="736" activeTab="1"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="25600" windowHeight="17520" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="13" r:id="rId1"/>
@@ -7205,6 +7205,97 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="amplicon.pptx.v2.f.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="13778" t="19161" r="12462" b="15625"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2654300"/>
+          <a:ext cx="7886700" cy="4927600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="amplicon.pptx.v2.r.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="14847" t="18657" r="12937" b="13944"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8039100" y="2628900"/>
+          <a:ext cx="7721600" cy="5092700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table246" displayName="Table246" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
@@ -9532,9 +9623,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>